<commit_message>
🔧 update reward type to terminal
</commit_message>
<xml_diff>
--- a/AdaptiveMarketPlanning/Base parameters.xlsx
+++ b/AdaptiveMarketPlanning/Base parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnascime/Dropbox/PythonProjects/ORF411/github_private/seqdecisionlib_Newsvendor/AdaptiveMarketPlanning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongjun-u/Documents/GitHub/IIE4124-Optimization-Theory-and-Application/AdaptiveMarketPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD22F369-1B04-7A40-98A0-FCC2FEE1E140}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A6EFB8-5C40-3842-8EC5-89007AF97181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="5840" windowWidth="17180" windowHeight="8780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>reward_type</t>
   </si>
   <si>
-    <t>Terminal</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Possible values for </t>
     </r>
@@ -58,7 +55,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -68,7 +65,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -81,7 +78,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -91,7 +88,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -104,7 +101,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -114,7 +111,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -124,30 +121,34 @@
   <si>
     <t>Whe the reward_type is "Cumulative" the reported average cumulative reward was divided by T (in order to be comparable to   the average terminal reward)</t>
   </si>
+  <si>
+    <t>Terminal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -155,7 +156,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -163,7 +164,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -171,35 +172,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -207,7 +208,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -215,14 +216,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -230,14 +231,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -245,7 +246,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -253,15 +254,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -611,48 +619,48 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="강조색1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="강조색2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="강조색3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="강조색4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="강조색5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="강조색6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="경고문" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="계산" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="나쁨" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="메모" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="보통" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="설명 텍스트" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="셀 확인" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="연결된 셀" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="요약" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="입력" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="제목" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="제목 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="제목 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="제목 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="제목 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="좋음" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,9 +676,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -708,7 +716,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -814,7 +822,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -956,7 +964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -970,29 +978,30 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1002,10 +1011,10 @@
   <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -1050,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3">
@@ -1066,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="3:3">
@@ -1076,6 +1085,7 @@
       <c r="C19" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>